<commit_message>
change pm consideration to "planning related gap"
</commit_message>
<xml_diff>
--- a/SiteStatusProject.xlsx
+++ b/SiteStatusProject.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programs\python\siteStatus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F71E7D93-734E-4923-8D37-0F47897E2BFF}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE34FFEC-4763-4558-9F69-9BDFB951B402}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SiteStatusProject" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">SiteStatusProject!$B$1:$B$258</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -34,10 +37,10 @@
     <t>Custom field (Mission start date/time)</t>
   </si>
   <si>
-    <t>Custom field (Fail key reason)</t>
+    <t>Custom field (Flight Cancellation Key Reason)</t>
   </si>
   <si>
-    <t>Custom field (Flight Cancellation Key Reason)</t>
+    <t>Custom field (Fail key reason)</t>
   </si>
   <si>
     <t>Created</t>
@@ -447,15 +450,15 @@
   <dimension ref="A1:G258"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="B76" sqref="B76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="32.26953125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="32.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.6328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="38.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.6328125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -971,7 +974,7 @@
       <c r="D30" s="1">
         <v>43244.424305555571</v>
       </c>
-      <c r="E30" t="s">
+      <c r="F30" t="s">
         <v>12</v>
       </c>
       <c r="G30" s="1">
@@ -1042,7 +1045,7 @@
       <c r="D34" s="1">
         <v>43245.570138888892</v>
       </c>
-      <c r="F34" t="s">
+      <c r="E34" t="s">
         <v>15</v>
       </c>
       <c r="G34" s="1">
@@ -1062,7 +1065,7 @@
       <c r="D35" s="1">
         <v>43244.570138888892</v>
       </c>
-      <c r="F35" t="s">
+      <c r="E35" t="s">
         <v>15</v>
       </c>
       <c r="G35" s="1">
@@ -1303,7 +1306,7 @@
       <c r="D49" s="1">
         <v>43244.46458333332</v>
       </c>
-      <c r="F49" t="s">
+      <c r="E49" t="s">
         <v>12</v>
       </c>
       <c r="G49" s="1">
@@ -1323,7 +1326,7 @@
       <c r="D50" s="1">
         <v>43244.462500000001</v>
       </c>
-      <c r="F50" t="s">
+      <c r="E50" t="s">
         <v>12</v>
       </c>
       <c r="G50" s="1">
@@ -1377,7 +1380,7 @@
       <c r="D53" s="1">
         <v>43242.661805555559</v>
       </c>
-      <c r="E53" t="s">
+      <c r="F53" t="s">
         <v>20</v>
       </c>
       <c r="G53" s="1">
@@ -1635,7 +1638,7 @@
       <c r="D68" s="1">
         <v>43242.363888888889</v>
       </c>
-      <c r="F68" t="s">
+      <c r="E68" t="s">
         <v>15</v>
       </c>
       <c r="G68" s="1">
@@ -1655,7 +1658,7 @@
       <c r="D69" s="1">
         <v>43242.354166666657</v>
       </c>
-      <c r="F69" t="s">
+      <c r="E69" t="s">
         <v>15</v>
       </c>
       <c r="G69" s="1">
@@ -1692,7 +1695,7 @@
       <c r="D71" s="1">
         <v>43245</v>
       </c>
-      <c r="F71" t="s">
+      <c r="E71" t="s">
         <v>15</v>
       </c>
       <c r="G71" s="1">
@@ -1712,7 +1715,7 @@
       <c r="D72" s="1">
         <v>43245.479166666657</v>
       </c>
-      <c r="F72" t="s">
+      <c r="E72" t="s">
         <v>15</v>
       </c>
       <c r="G72" s="1">
@@ -1749,7 +1752,7 @@
       <c r="D74" s="1">
         <v>43245.479166666657</v>
       </c>
-      <c r="F74" t="s">
+      <c r="E74" t="s">
         <v>21</v>
       </c>
       <c r="G74" s="1">
@@ -1769,7 +1772,7 @@
       <c r="D75" s="1">
         <v>43244.479166666657</v>
       </c>
-      <c r="F75" t="s">
+      <c r="E75" t="s">
         <v>15</v>
       </c>
       <c r="G75" s="1">
@@ -1891,7 +1894,7 @@
       <c r="D82" s="1">
         <v>43241.010416666657</v>
       </c>
-      <c r="F82" t="s">
+      <c r="E82" t="s">
         <v>21</v>
       </c>
       <c r="G82" s="1">
@@ -1911,7 +1914,7 @@
       <c r="D83" s="1">
         <v>43242.298611111109</v>
       </c>
-      <c r="F83" t="s">
+      <c r="E83" t="s">
         <v>23</v>
       </c>
       <c r="G83" s="1">
@@ -1999,7 +2002,7 @@
       <c r="D88" s="1">
         <v>43244.010416666657</v>
       </c>
-      <c r="F88" t="s">
+      <c r="E88" t="s">
         <v>15</v>
       </c>
       <c r="G88" s="1">
@@ -2019,7 +2022,7 @@
       <c r="D89" s="1">
         <v>43244.479166666657</v>
       </c>
-      <c r="F89" t="s">
+      <c r="E89" t="s">
         <v>15</v>
       </c>
       <c r="G89" s="1">
@@ -2141,7 +2144,7 @@
       <c r="D96" s="1">
         <v>43243.375</v>
       </c>
-      <c r="E96" t="s">
+      <c r="F96" t="s">
         <v>20</v>
       </c>
       <c r="G96" s="1">
@@ -2161,7 +2164,7 @@
       <c r="D97" s="1">
         <v>43243.375</v>
       </c>
-      <c r="E97" t="s">
+      <c r="F97" t="s">
         <v>20</v>
       </c>
       <c r="G97" s="1">
@@ -2181,7 +2184,7 @@
       <c r="D98" s="1">
         <v>43245.010416666657</v>
       </c>
-      <c r="F98" t="s">
+      <c r="E98" t="s">
         <v>21</v>
       </c>
       <c r="G98" s="1">
@@ -2201,7 +2204,7 @@
       <c r="D99" s="1">
         <v>43244.010416666657</v>
       </c>
-      <c r="F99" t="s">
+      <c r="E99" t="s">
         <v>21</v>
       </c>
       <c r="G99" s="1">
@@ -2221,7 +2224,7 @@
       <c r="D100" s="1">
         <v>43243.010416666657</v>
       </c>
-      <c r="F100" t="s">
+      <c r="E100" t="s">
         <v>20</v>
       </c>
       <c r="G100" s="1">
@@ -2241,7 +2244,7 @@
       <c r="D101" s="1">
         <v>43242.010416666657</v>
       </c>
-      <c r="F101" t="s">
+      <c r="E101" t="s">
         <v>21</v>
       </c>
       <c r="G101" s="1">
@@ -2261,7 +2264,7 @@
       <c r="D102" s="1">
         <v>43241.010416666657</v>
       </c>
-      <c r="F102" t="s">
+      <c r="E102" t="s">
         <v>21</v>
       </c>
       <c r="G102" s="1">
@@ -2298,7 +2301,7 @@
       <c r="D104" s="1">
         <v>43245.447916666657</v>
       </c>
-      <c r="F104" t="s">
+      <c r="E104" t="s">
         <v>21</v>
       </c>
       <c r="G104" s="1">
@@ -2318,7 +2321,7 @@
       <c r="D105" s="1">
         <v>43244.447916666657</v>
       </c>
-      <c r="F105" t="s">
+      <c r="E105" t="s">
         <v>21</v>
       </c>
       <c r="G105" s="1">
@@ -2338,7 +2341,7 @@
       <c r="D106" s="1">
         <v>43243.447916666657</v>
       </c>
-      <c r="F106" t="s">
+      <c r="E106" t="s">
         <v>21</v>
       </c>
       <c r="G106" s="1">
@@ -2358,7 +2361,7 @@
       <c r="D107" s="1">
         <v>43242.447916666657</v>
       </c>
-      <c r="F107" t="s">
+      <c r="E107" t="s">
         <v>21</v>
       </c>
       <c r="G107" s="1">
@@ -2378,7 +2381,7 @@
       <c r="D108" s="1">
         <v>43241.447916666657</v>
       </c>
-      <c r="F108" t="s">
+      <c r="E108" t="s">
         <v>21</v>
       </c>
       <c r="G108" s="1">
@@ -2415,7 +2418,7 @@
       <c r="D110" s="1">
         <v>43245.479166666657</v>
       </c>
-      <c r="F110" t="s">
+      <c r="E110" t="s">
         <v>21</v>
       </c>
       <c r="G110" s="1">
@@ -2435,7 +2438,7 @@
       <c r="D111" s="1">
         <v>43244.479166666657</v>
       </c>
-      <c r="F111" t="s">
+      <c r="E111" t="s">
         <v>21</v>
       </c>
       <c r="G111" s="1">
@@ -2455,7 +2458,7 @@
       <c r="D112" s="1">
         <v>43243.479166666657</v>
       </c>
-      <c r="F112" t="s">
+      <c r="E112" t="s">
         <v>21</v>
       </c>
       <c r="G112" s="1">
@@ -2475,7 +2478,7 @@
       <c r="D113" s="1">
         <v>43242.479166666657</v>
       </c>
-      <c r="F113" t="s">
+      <c r="E113" t="s">
         <v>21</v>
       </c>
       <c r="G113" s="1">
@@ -2495,7 +2498,7 @@
       <c r="D114" s="1">
         <v>43241.479166666657</v>
       </c>
-      <c r="F114" t="s">
+      <c r="E114" t="s">
         <v>21</v>
       </c>
       <c r="G114" s="1">
@@ -2532,7 +2535,7 @@
       <c r="D116" s="1">
         <v>43244.347222222219</v>
       </c>
-      <c r="F116" t="s">
+      <c r="E116" t="s">
         <v>15</v>
       </c>
       <c r="G116" s="1">
@@ -2552,7 +2555,7 @@
       <c r="D117" s="1">
         <v>43244.34375</v>
       </c>
-      <c r="F117" t="s">
+      <c r="E117" t="s">
         <v>15</v>
       </c>
       <c r="G117" s="1">
@@ -2606,7 +2609,7 @@
       <c r="D120" s="1">
         <v>43243.395833333343</v>
       </c>
-      <c r="E120" t="s">
+      <c r="F120" t="s">
         <v>20</v>
       </c>
       <c r="G120" s="1">
@@ -2660,7 +2663,7 @@
       <c r="D123" s="1">
         <v>43243.354166666657</v>
       </c>
-      <c r="E123" t="s">
+      <c r="F123" t="s">
         <v>20</v>
       </c>
       <c r="G123" s="1">
@@ -2765,7 +2768,7 @@
       <c r="D129" s="1">
         <v>43241.145833333343</v>
       </c>
-      <c r="F129" t="s">
+      <c r="E129" t="s">
         <v>15</v>
       </c>
       <c r="G129" s="1">
@@ -2785,7 +2788,7 @@
       <c r="D130" s="1">
         <v>43241.145833333343</v>
       </c>
-      <c r="F130" t="s">
+      <c r="E130" t="s">
         <v>15</v>
       </c>
       <c r="G130" s="1">
@@ -2805,7 +2808,7 @@
       <c r="D131" s="1">
         <v>43241.145833333343</v>
       </c>
-      <c r="F131" t="s">
+      <c r="E131" t="s">
         <v>15</v>
       </c>
       <c r="G131" s="1">
@@ -2825,7 +2828,7 @@
       <c r="D132" s="1">
         <v>43240.375</v>
       </c>
-      <c r="F132" t="s">
+      <c r="E132" t="s">
         <v>15</v>
       </c>
       <c r="G132" s="1">
@@ -2845,7 +2848,7 @@
       <c r="D133" s="1">
         <v>43240.375</v>
       </c>
-      <c r="F133" t="s">
+      <c r="E133" t="s">
         <v>15</v>
       </c>
       <c r="G133" s="1">
@@ -2865,7 +2868,7 @@
       <c r="D134" s="1">
         <v>43240.375</v>
       </c>
-      <c r="F134" t="s">
+      <c r="E134" t="s">
         <v>15</v>
       </c>
       <c r="G134" s="1">
@@ -2885,7 +2888,7 @@
       <c r="D135" s="1">
         <v>43245.375</v>
       </c>
-      <c r="F135" t="s">
+      <c r="E135" t="s">
         <v>23</v>
       </c>
       <c r="G135" s="1">
@@ -2905,7 +2908,7 @@
       <c r="D136" s="1">
         <v>43242.375</v>
       </c>
-      <c r="F136" t="s">
+      <c r="E136" t="s">
         <v>15</v>
       </c>
       <c r="G136" s="1">
@@ -2959,7 +2962,7 @@
       <c r="D139" s="1">
         <v>43241.375</v>
       </c>
-      <c r="F139" t="s">
+      <c r="E139" t="s">
         <v>15</v>
       </c>
       <c r="G139" s="1">
@@ -2979,7 +2982,7 @@
       <c r="D140" s="1">
         <v>43240.375</v>
       </c>
-      <c r="F140" t="s">
+      <c r="E140" t="s">
         <v>15</v>
       </c>
       <c r="G140" s="1">
@@ -2999,7 +3002,7 @@
       <c r="D141" s="1">
         <v>43241.375</v>
       </c>
-      <c r="F141" t="s">
+      <c r="E141" t="s">
         <v>15</v>
       </c>
       <c r="G141" s="1">
@@ -3104,7 +3107,7 @@
       <c r="D147" s="1">
         <v>43245.399305555547</v>
       </c>
-      <c r="F147" t="s">
+      <c r="E147" t="s">
         <v>15</v>
       </c>
       <c r="G147" s="1">
@@ -3124,7 +3127,7 @@
       <c r="D148" s="1">
         <v>43245.397916666669</v>
       </c>
-      <c r="F148" t="s">
+      <c r="E148" t="s">
         <v>15</v>
       </c>
       <c r="G148" s="1">
@@ -3144,7 +3147,7 @@
       <c r="D149" s="1">
         <v>43244.399305555547</v>
       </c>
-      <c r="F149" t="s">
+      <c r="E149" t="s">
         <v>15</v>
       </c>
       <c r="G149" s="1">
@@ -3283,7 +3286,7 @@
       <c r="D157" s="1">
         <v>43245.569444444453</v>
       </c>
-      <c r="F157" t="s">
+      <c r="E157" t="s">
         <v>15</v>
       </c>
       <c r="G157" s="1">
@@ -3303,7 +3306,7 @@
       <c r="D158" s="1">
         <v>43244.569444444453</v>
       </c>
-      <c r="F158" t="s">
+      <c r="E158" t="s">
         <v>15</v>
       </c>
       <c r="G158" s="1">
@@ -3357,7 +3360,7 @@
       <c r="D161" s="1">
         <v>43241.569444444453</v>
       </c>
-      <c r="F161" t="s">
+      <c r="E161" t="s">
         <v>20</v>
       </c>
       <c r="G161" s="1">
@@ -3377,7 +3380,7 @@
       <c r="D162" s="1">
         <v>43245.578472222223</v>
       </c>
-      <c r="F162" t="s">
+      <c r="E162" t="s">
         <v>15</v>
       </c>
       <c r="G162" s="1">
@@ -3431,7 +3434,7 @@
       <c r="D165" s="1">
         <v>43242.578472222223</v>
       </c>
-      <c r="E165" t="s">
+      <c r="F165" t="s">
         <v>20</v>
       </c>
       <c r="G165" s="1">
@@ -3468,7 +3471,7 @@
       <c r="D167" s="1">
         <v>43245.511111111111</v>
       </c>
-      <c r="F167" t="s">
+      <c r="E167" t="s">
         <v>15</v>
       </c>
       <c r="G167" s="1">
@@ -3488,7 +3491,7 @@
       <c r="D168" s="1">
         <v>43244.511111111111</v>
       </c>
-      <c r="F168" t="s">
+      <c r="E168" t="s">
         <v>15</v>
       </c>
       <c r="G168" s="1">
@@ -3542,7 +3545,7 @@
       <c r="D171" s="1">
         <v>43241.511111111111</v>
       </c>
-      <c r="F171" t="s">
+      <c r="E171" t="s">
         <v>20</v>
       </c>
       <c r="G171" s="1">
@@ -3630,7 +3633,7 @@
       <c r="D176" s="1">
         <v>43240.319444444453</v>
       </c>
-      <c r="F176" t="s">
+      <c r="E176" t="s">
         <v>21</v>
       </c>
       <c r="G176" s="1">
@@ -3735,7 +3738,7 @@
       <c r="D182" s="1">
         <v>43239.864583333343</v>
       </c>
-      <c r="F182" t="s">
+      <c r="E182" t="s">
         <v>20</v>
       </c>
       <c r="G182" s="1">
@@ -3772,7 +3775,7 @@
       <c r="D184" s="1">
         <v>43243.819444444453</v>
       </c>
-      <c r="F184" t="s">
+      <c r="E184" t="s">
         <v>23</v>
       </c>
       <c r="G184" s="1">
@@ -3809,7 +3812,7 @@
       <c r="D186" s="1">
         <v>43241.819444444453</v>
       </c>
-      <c r="F186" t="s">
+      <c r="E186" t="s">
         <v>23</v>
       </c>
       <c r="G186" s="1">
@@ -3863,7 +3866,7 @@
       <c r="D189" s="1">
         <v>43242.708333333343</v>
       </c>
-      <c r="E189" t="s">
+      <c r="F189" t="s">
         <v>12</v>
       </c>
       <c r="G189" s="1">
@@ -3985,7 +3988,7 @@
       <c r="D196" s="1">
         <v>43241.864583333343</v>
       </c>
-      <c r="F196" t="s">
+      <c r="E196" t="s">
         <v>23</v>
       </c>
       <c r="G196" s="1">
@@ -4005,7 +4008,7 @@
       <c r="D197" s="1">
         <v>43240.364583333343</v>
       </c>
-      <c r="F197" t="s">
+      <c r="E197" t="s">
         <v>21</v>
       </c>
       <c r="G197" s="1">
@@ -4059,7 +4062,7 @@
       <c r="D200" s="1">
         <v>43241.520833333343</v>
       </c>
-      <c r="F200" t="s">
+      <c r="E200" t="s">
         <v>23</v>
       </c>
       <c r="G200" s="1">
@@ -4079,7 +4082,7 @@
       <c r="D201" s="1">
         <v>43240.520833333343</v>
       </c>
-      <c r="F201" t="s">
+      <c r="E201" t="s">
         <v>21</v>
       </c>
       <c r="G201" s="1">
@@ -4167,7 +4170,7 @@
       <c r="D206" s="1">
         <v>43240.270833333343</v>
       </c>
-      <c r="F206" t="s">
+      <c r="E206" t="s">
         <v>21</v>
       </c>
       <c r="G206" s="1">
@@ -4187,7 +4190,7 @@
       <c r="D207" s="1">
         <v>43245.572916666657</v>
       </c>
-      <c r="F207" t="s">
+      <c r="E207" t="s">
         <v>21</v>
       </c>
       <c r="G207" s="1">
@@ -4207,7 +4210,7 @@
       <c r="D208" s="1">
         <v>43244.572916666657</v>
       </c>
-      <c r="F208" t="s">
+      <c r="E208" t="s">
         <v>15</v>
       </c>
       <c r="G208" s="1">
@@ -4227,7 +4230,7 @@
       <c r="D209" s="1">
         <v>43243.572916666657</v>
       </c>
-      <c r="F209" t="s">
+      <c r="E209" t="s">
         <v>21</v>
       </c>
       <c r="G209" s="1">
@@ -4247,7 +4250,7 @@
       <c r="D210" s="1">
         <v>43242.572916666657</v>
       </c>
-      <c r="F210" t="s">
+      <c r="E210" t="s">
         <v>21</v>
       </c>
       <c r="G210" s="1">
@@ -4267,7 +4270,7 @@
       <c r="D211" s="1">
         <v>43241.572916666657</v>
       </c>
-      <c r="F211" t="s">
+      <c r="E211" t="s">
         <v>21</v>
       </c>
       <c r="G211" s="1">
@@ -4287,7 +4290,7 @@
       <c r="D212" s="1">
         <v>43240.572916666657</v>
       </c>
-      <c r="F212" t="s">
+      <c r="E212" t="s">
         <v>21</v>
       </c>
       <c r="G212" s="1">
@@ -4307,7 +4310,7 @@
       <c r="D213" s="1">
         <v>43241.572916666657</v>
       </c>
-      <c r="F213" t="s">
+      <c r="E213" t="s">
         <v>21</v>
       </c>
       <c r="G213" s="1">
@@ -4327,7 +4330,7 @@
       <c r="D214" s="1">
         <v>43245.541666666657</v>
       </c>
-      <c r="F214" t="s">
+      <c r="E214" t="s">
         <v>21</v>
       </c>
       <c r="G214" s="1">
@@ -4347,7 +4350,7 @@
       <c r="D215" s="1">
         <v>43244.541666666657</v>
       </c>
-      <c r="F215" t="s">
+      <c r="E215" t="s">
         <v>21</v>
       </c>
       <c r="G215" s="1">
@@ -4367,7 +4370,7 @@
       <c r="D216" s="1">
         <v>43243.541666666657</v>
       </c>
-      <c r="F216" t="s">
+      <c r="E216" t="s">
         <v>21</v>
       </c>
       <c r="G216" s="1">
@@ -4387,7 +4390,7 @@
       <c r="D217" s="1">
         <v>43242.541666666657</v>
       </c>
-      <c r="F217" t="s">
+      <c r="E217" t="s">
         <v>21</v>
       </c>
       <c r="G217" s="1">
@@ -4407,7 +4410,7 @@
       <c r="D218" s="1">
         <v>43241.541666666657</v>
       </c>
-      <c r="F218" t="s">
+      <c r="E218" t="s">
         <v>21</v>
       </c>
       <c r="G218" s="1">
@@ -4427,7 +4430,7 @@
       <c r="D219" s="1">
         <v>43240.541666666657</v>
       </c>
-      <c r="F219" t="s">
+      <c r="E219" t="s">
         <v>21</v>
       </c>
       <c r="G219" s="1">
@@ -4447,7 +4450,7 @@
       <c r="D220" s="1">
         <v>43245.010416666657</v>
       </c>
-      <c r="F220" t="s">
+      <c r="E220" t="s">
         <v>15</v>
       </c>
       <c r="G220" s="1">
@@ -4467,7 +4470,7 @@
       <c r="D221" s="1">
         <v>43244.010416666657</v>
       </c>
-      <c r="F221" t="s">
+      <c r="E221" t="s">
         <v>21</v>
       </c>
       <c r="G221" s="1">
@@ -4521,7 +4524,7 @@
       <c r="D224" s="1">
         <v>43241.010416666657</v>
       </c>
-      <c r="F224" t="s">
+      <c r="E224" t="s">
         <v>21</v>
       </c>
       <c r="G224" s="1">
@@ -4558,7 +4561,7 @@
       <c r="D226" s="1">
         <v>43245.479166666657</v>
       </c>
-      <c r="F226" t="s">
+      <c r="E226" t="s">
         <v>15</v>
       </c>
       <c r="G226" s="1">
@@ -4578,7 +4581,7 @@
       <c r="D227" s="1">
         <v>43244.479166666657</v>
       </c>
-      <c r="F227" t="s">
+      <c r="E227" t="s">
         <v>21</v>
       </c>
       <c r="G227" s="1">
@@ -4598,7 +4601,7 @@
       <c r="D228" s="1">
         <v>43243.479166666657</v>
       </c>
-      <c r="F228" t="s">
+      <c r="E228" t="s">
         <v>20</v>
       </c>
       <c r="G228" s="1">
@@ -4635,7 +4638,7 @@
       <c r="D230" s="1">
         <v>43241.479166666657</v>
       </c>
-      <c r="F230" t="s">
+      <c r="E230" t="s">
         <v>21</v>
       </c>
       <c r="G230" s="1">
@@ -4672,7 +4675,7 @@
       <c r="D232" s="1">
         <v>43245.486805555571</v>
       </c>
-      <c r="F232" t="s">
+      <c r="E232" t="s">
         <v>15</v>
       </c>
       <c r="G232" s="1">
@@ -4743,7 +4746,7 @@
       <c r="D236" s="1">
         <v>43241.491666666669</v>
       </c>
-      <c r="F236" t="s">
+      <c r="E236" t="s">
         <v>20</v>
       </c>
       <c r="G236" s="1">
@@ -4797,7 +4800,7 @@
       <c r="D239" s="1">
         <v>43241.479166666657</v>
       </c>
-      <c r="F239" t="s">
+      <c r="E239" t="s">
         <v>23</v>
       </c>
       <c r="G239" s="1">
@@ -4817,7 +4820,7 @@
       <c r="D240" s="1">
         <v>43242.479166666657</v>
       </c>
-      <c r="F240" t="s">
+      <c r="E240" t="s">
         <v>21</v>
       </c>
       <c r="G240" s="1">
@@ -4837,7 +4840,7 @@
       <c r="D241" s="1">
         <v>43243.479166666657</v>
       </c>
-      <c r="F241" t="s">
+      <c r="E241" t="s">
         <v>21</v>
       </c>
       <c r="G241" s="1">
@@ -4857,7 +4860,7 @@
       <c r="D242" s="1">
         <v>43244.479166666657</v>
       </c>
-      <c r="F242" t="s">
+      <c r="E242" t="s">
         <v>21</v>
       </c>
       <c r="G242" s="1">
@@ -4877,7 +4880,7 @@
       <c r="D243" s="1">
         <v>43245.479166666657</v>
       </c>
-      <c r="F243" t="s">
+      <c r="E243" t="s">
         <v>21</v>
       </c>
       <c r="G243" s="1">
@@ -4897,7 +4900,7 @@
       <c r="D244" s="1">
         <v>43245.447916666657</v>
       </c>
-      <c r="F244" t="s">
+      <c r="E244" t="s">
         <v>21</v>
       </c>
       <c r="G244" s="1">
@@ -4917,7 +4920,7 @@
       <c r="D245" s="1">
         <v>43244.447916666657</v>
       </c>
-      <c r="F245" t="s">
+      <c r="E245" t="s">
         <v>21</v>
       </c>
       <c r="G245" s="1">
@@ -4937,7 +4940,7 @@
       <c r="D246" s="1">
         <v>43243.447916666657</v>
       </c>
-      <c r="F246" t="s">
+      <c r="E246" t="s">
         <v>21</v>
       </c>
       <c r="G246" s="1">
@@ -4957,7 +4960,7 @@
       <c r="D247" s="1">
         <v>43242.447916666657</v>
       </c>
-      <c r="F247" t="s">
+      <c r="E247" t="s">
         <v>21</v>
       </c>
       <c r="G247" s="1">
@@ -5011,7 +5014,7 @@
       <c r="D250" s="1">
         <v>43245.416666666657</v>
       </c>
-      <c r="F250" t="s">
+      <c r="E250" t="s">
         <v>21</v>
       </c>
       <c r="G250" s="1">
@@ -5031,7 +5034,7 @@
       <c r="D251" s="1">
         <v>43244.416666666657</v>
       </c>
-      <c r="F251" t="s">
+      <c r="E251" t="s">
         <v>21</v>
       </c>
       <c r="G251" s="1">
@@ -5051,7 +5054,7 @@
       <c r="D252" s="1">
         <v>43243.416666666657</v>
       </c>
-      <c r="F252" t="s">
+      <c r="E252" t="s">
         <v>21</v>
       </c>
       <c r="G252" s="1">
@@ -5071,7 +5074,7 @@
       <c r="D253" s="1">
         <v>43242.416666666657</v>
       </c>
-      <c r="F253" t="s">
+      <c r="E253" t="s">
         <v>21</v>
       </c>
       <c r="G253" s="1">
@@ -5108,7 +5111,7 @@
       <c r="D255" s="1">
         <v>43245.491666666669</v>
       </c>
-      <c r="F255" t="s">
+      <c r="E255" t="s">
         <v>15</v>
       </c>
       <c r="G255" s="1">
@@ -5167,6 +5170,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="B1:B258" xr:uid="{BE931607-383C-4A21-8AD1-0D4840D023AC}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>